<commit_message>
update pip parameters template
</commit_message>
<xml_diff>
--- a/Proposed/Adding_An_Index/PIP_TEMPLATE/Set_Drop.xlsx
+++ b/Proposed/Adding_An_Index/PIP_TEMPLATE/Set_Drop.xlsx
@@ -519,10 +519,10 @@
         <v>2.641E-5</v>
       </c>
       <c r="D2" s="5">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E2" s="5">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="F2" s="4">
         <f>0.2/(A2*3)</f>
@@ -634,12 +634,12 @@
     </row>
     <row r="12">
       <c r="A12" s="12">
-        <f>D2+(F2*A2)</f>
-        <v>0.4666666667</v>
+        <f>IF(D2+(F2*A2)&lt;=E2,D2+(F2*A2),E2)</f>
+        <v>0.8666666667</v>
       </c>
       <c r="B12" s="12">
         <f>E2-(F2*A2)</f>
-        <v>0.5333333333</v>
+        <v>0.8833333333</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -675,7 +675,7 @@
     <row r="16">
       <c r="A16" s="12">
         <f>C8/A12</f>
-        <v>4047.501277</v>
+        <v>2179.423765</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -704,7 +704,7 @@
     <row r="19">
       <c r="A19" s="12">
         <f>A16/A2</f>
-        <v>1.12430591</v>
+        <v>0.6053954901</v>
       </c>
       <c r="B19" s="12" t="str">
         <f>CONCATENATE(B2, " Tokens per a second")</f>
@@ -736,7 +736,7 @@
     <row r="22">
       <c r="A22" s="13">
         <f>A19*(10^B4)</f>
-        <v>1.12431E+18</v>
+        <v>6.05395E+17</v>
       </c>
       <c r="B22" s="12" t="str">
         <f>B19</f>

</xml_diff>